<commit_message>
Changed load cell termination pads
</commit_message>
<xml_diff>
--- a/ProjectOutputs/LoadCellAmplifier-Workbook.xlsx
+++ b/ProjectOutputs/LoadCellAmplifier-Workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38920" yWindow="-980" windowWidth="20960" windowHeight="20400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="38700" yWindow="-1120" windowWidth="15100" windowHeight="23260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wheatsone Bridge" sheetId="1" r:id="rId1"/>
@@ -938,10 +938,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1062,27 +1062,27 @@
         <v>3.74</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" ref="E6:E15" si="0">B6+E$4</f>
+        <f t="shared" ref="E6:E18" si="0">B6+E$4</f>
         <v>4.6300000000000008</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" ref="F6:F15" si="1">C6</f>
+        <f t="shared" ref="F6:F18" si="1">C6</f>
         <v>3.74</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" ref="H6:H15" si="2">E6+H$4</f>
+        <f t="shared" ref="H6:H18" si="2">E6+H$4</f>
         <v>5.15</v>
       </c>
       <c r="I6" s="5">
-        <f t="shared" ref="I6:I15" si="3">F6</f>
+        <f t="shared" ref="I6:I18" si="3">F6</f>
         <v>3.74</v>
       </c>
       <c r="K6" s="5">
-        <f t="shared" ref="K6:K15" si="4">H6+K$4</f>
+        <f t="shared" ref="K6:K18" si="4">H6+K$4</f>
         <v>5.67</v>
       </c>
       <c r="L6" s="5">
-        <f t="shared" ref="L6:L15" si="5">I6</f>
+        <f t="shared" ref="L6:L18" si="5">I6</f>
         <v>3.74</v>
       </c>
     </row>
@@ -1156,85 +1156,61 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:12" ht="6" customHeight="1">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B10" s="6">
         <v>4.1100000000000003</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C10" s="6">
         <v>3.5760000000000001</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E10" s="5">
         <f t="shared" si="0"/>
         <v>4.6300000000000008</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F10" s="5">
         <f t="shared" si="1"/>
         <v>3.5760000000000001</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H10" s="5">
         <f t="shared" si="2"/>
         <v>5.15</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I10" s="5">
         <f t="shared" si="3"/>
         <v>3.5760000000000001</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K10" s="5">
         <f t="shared" si="4"/>
         <v>5.67</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L10" s="5">
         <f t="shared" si="5"/>
         <v>3.5760000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="6">
-        <v>4.2389999999999999</v>
-      </c>
-      <c r="C10" s="6">
-        <v>3.7309999999999999</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>4.7590000000000003</v>
-      </c>
-      <c r="F10" s="5">
-        <f t="shared" si="1"/>
-        <v>3.7309999999999999</v>
-      </c>
-      <c r="H10" s="5">
-        <f t="shared" si="2"/>
-        <v>5.2789999999999999</v>
-      </c>
-      <c r="I10" s="5">
-        <f t="shared" si="3"/>
-        <v>3.7309999999999999</v>
-      </c>
-      <c r="K10" s="5">
-        <f t="shared" si="4"/>
-        <v>5.7989999999999995</v>
-      </c>
-      <c r="L10" s="5">
-        <f t="shared" si="5"/>
-        <v>3.7309999999999999</v>
-      </c>
-    </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6">
         <v>4.2389999999999999</v>
       </c>
-      <c r="C11" s="7">
-        <v>3.5960000000000001</v>
+      <c r="C11" s="6">
+        <v>3.7309999999999999</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="0"/>
@@ -1242,7 +1218,7 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="1"/>
-        <v>3.5960000000000001</v>
+        <v>3.7309999999999999</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="2"/>
@@ -1250,7 +1226,7 @@
       </c>
       <c r="I11" s="5">
         <f t="shared" si="3"/>
-        <v>3.5960000000000001</v>
+        <v>3.7309999999999999</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="4"/>
@@ -1258,145 +1234,202 @@
       </c>
       <c r="L11" s="5">
         <f t="shared" si="5"/>
+        <v>3.7309999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="6" customHeight="1">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6">
+        <v>4.2389999999999999</v>
+      </c>
+      <c r="C13" s="7">
         <v>3.5960000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1" t="s">
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>4.7590000000000003</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>3.5960000000000001</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="2"/>
+        <v>5.2789999999999999</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="3"/>
+        <v>3.5960000000000001</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="4"/>
+        <v>5.7989999999999995</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="5"/>
+        <v>3.5960000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="6" customHeight="1">
+      <c r="A14" s="1"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B15" s="6">
         <v>4.3949999999999996</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C15" s="6">
         <v>3.831</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E15" s="5">
         <f t="shared" si="0"/>
         <v>4.9149999999999991</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F15" s="5">
         <f t="shared" si="1"/>
         <v>3.831</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H15" s="5">
         <f t="shared" si="2"/>
         <v>5.4349999999999987</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I15" s="5">
         <f t="shared" si="3"/>
         <v>3.831</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K15" s="5">
         <f t="shared" si="4"/>
         <v>5.9549999999999983</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L15" s="5">
         <f t="shared" si="5"/>
         <v>3.831</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="1" t="s">
+    <row r="16" spans="1:12">
+      <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B16" s="7">
         <v>4.3</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C16" s="7">
         <v>3.831</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E16" s="5">
         <f t="shared" si="0"/>
         <v>4.82</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F16" s="5">
         <f t="shared" si="1"/>
         <v>3.831</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H16" s="5">
         <f t="shared" si="2"/>
         <v>5.34</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I16" s="5">
         <f t="shared" si="3"/>
         <v>3.831</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K16" s="5">
         <f t="shared" si="4"/>
         <v>5.8599999999999994</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L16" s="5">
         <f t="shared" si="5"/>
         <v>3.831</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="1" t="s">
+    <row r="17" spans="1:12">
+      <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B17" s="6">
         <v>4.3470000000000004</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C17" s="6">
         <v>3.6139999999999999</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E17" s="5">
         <f t="shared" si="0"/>
         <v>4.8670000000000009</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F17" s="5">
         <f t="shared" si="1"/>
         <v>3.6139999999999999</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H17" s="5">
         <f t="shared" si="2"/>
         <v>5.3870000000000005</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I17" s="5">
         <f t="shared" si="3"/>
         <v>3.6139999999999999</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K17" s="5">
         <f t="shared" si="4"/>
         <v>5.907</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L17" s="5">
         <f t="shared" si="5"/>
         <v>3.6139999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="1" t="s">
+    <row r="18" spans="1:12">
+      <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B18" s="6">
         <v>4.3470000000000004</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C18" s="7">
         <v>3.5649999999999999</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E18" s="5">
         <f t="shared" si="0"/>
         <v>4.8670000000000009</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F18" s="5">
         <f t="shared" si="1"/>
         <v>3.5649999999999999</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H18" s="5">
         <f t="shared" si="2"/>
         <v>5.3870000000000005</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I18" s="5">
         <f t="shared" si="3"/>
         <v>3.5649999999999999</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K18" s="5">
         <f t="shared" si="4"/>
         <v>5.907</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L18" s="5">
         <f t="shared" si="5"/>
         <v>3.5649999999999999</v>
       </c>

</xml_diff>

<commit_message>
Added fiducials, final check
</commit_message>
<xml_diff>
--- a/ProjectOutputs/LoadCellAmplifier-Workbook.xlsx
+++ b/ProjectOutputs/LoadCellAmplifier-Workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38700" yWindow="-1120" windowWidth="15100" windowHeight="23260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wheatsone Bridge" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Wheatstone bridge like so:</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>(Offset)</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>inches</t>
+  </si>
+  <si>
+    <t>Mousebites</t>
   </si>
 </sst>
 </file>
@@ -167,8 +176,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -217,14 +232,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -243,6 +258,9 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -261,6 +279,9 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -786,10 +807,10 @@
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="2:4">
       <c r="C6" s="3" t="s">
@@ -816,10 +837,10 @@
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
@@ -897,7 +918,7 @@
       <c r="B22" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <f>C16*(C18/(C17+C18))</f>
         <v>6.0150375939849621</v>
       </c>
@@ -906,7 +927,7 @@
       <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <f>C16*(C20/(C19+C20))</f>
         <v>6</v>
       </c>
@@ -915,7 +936,7 @@
       <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <f>C22-C23</f>
         <v>1.5037593984962072E-2</v>
       </c>
@@ -938,10 +959,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1003,15 +1024,15 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0.52</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>0.52</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>0.52</v>
       </c>
       <c r="L4" s="1"/>
@@ -1020,33 +1041,33 @@
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>4.22</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>3.93</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <f>B5+E$4</f>
         <v>4.74</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f>C5</f>
         <v>3.93</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <f>E5+H$4</f>
         <v>5.26</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <f>F5</f>
         <v>3.93</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <f>H5+K$4</f>
         <v>5.7799999999999994</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <f>I5</f>
         <v>3.93</v>
       </c>
@@ -1055,33 +1076,33 @@
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>4.1100000000000003</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>3.74</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <f t="shared" ref="E6:E18" si="0">B6+E$4</f>
         <v>4.6300000000000008</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f t="shared" ref="F6:F18" si="1">C6</f>
         <v>3.74</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <f t="shared" ref="H6:H18" si="2">E6+H$4</f>
         <v>5.15</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <f t="shared" ref="I6:I18" si="3">F6</f>
         <v>3.74</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <f t="shared" ref="K6:K18" si="4">H6+K$4</f>
         <v>5.67</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <f t="shared" ref="L6:L18" si="5">I6</f>
         <v>3.74</v>
       </c>
@@ -1090,33 +1111,33 @@
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>4.3470000000000004</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>3.7229999999999999</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f t="shared" si="0"/>
         <v>4.8670000000000009</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f t="shared" si="1"/>
         <v>3.7229999999999999</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <f t="shared" si="2"/>
         <v>5.3870000000000005</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <f t="shared" si="3"/>
         <v>3.7229999999999999</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <f t="shared" si="4"/>
         <v>5.907</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <f t="shared" si="5"/>
         <v>3.7229999999999999</v>
       </c>
@@ -1125,79 +1146,79 @@
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>4.2249999999999996</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>3.4</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f t="shared" si="0"/>
         <v>4.7449999999999992</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f t="shared" si="1"/>
         <v>3.4</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <f t="shared" si="2"/>
         <v>5.2649999999999988</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <f t="shared" si="3"/>
         <v>3.4</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <f t="shared" si="4"/>
         <v>5.7849999999999984</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <f t="shared" si="5"/>
         <v>3.4</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="6" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>4.1100000000000003</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>3.5760000000000001</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>4.6300000000000008</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
         <v>3.5760000000000001</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <f t="shared" si="2"/>
         <v>5.15</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <f t="shared" si="3"/>
         <v>3.5760000000000001</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="4">
         <f t="shared" si="4"/>
         <v>5.67</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="4">
         <f t="shared" si="5"/>
         <v>3.5760000000000001</v>
       </c>
@@ -1206,125 +1227,125 @@
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>4.2389999999999999</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>3.7309999999999999</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <f t="shared" si="0"/>
         <v>4.7590000000000003</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
         <v>3.7309999999999999</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <f t="shared" si="2"/>
         <v>5.2789999999999999</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <f t="shared" si="3"/>
         <v>3.7309999999999999</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <f t="shared" si="4"/>
         <v>5.7989999999999995</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="4">
         <f t="shared" si="5"/>
         <v>3.7309999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="6" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>4.2389999999999999</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>3.5960000000000001</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f t="shared" si="0"/>
         <v>4.7590000000000003</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f t="shared" si="1"/>
         <v>3.5960000000000001</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <f t="shared" si="2"/>
         <v>5.2789999999999999</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <f t="shared" si="3"/>
         <v>3.5960000000000001</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="4">
         <f t="shared" si="4"/>
         <v>5.7989999999999995</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <f t="shared" si="5"/>
         <v>3.5960000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="6" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>4.3949999999999996</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>3.831</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f t="shared" si="0"/>
         <v>4.9149999999999991</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <f t="shared" si="1"/>
         <v>3.831</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <f t="shared" si="2"/>
         <v>5.4349999999999987</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="4">
         <f t="shared" si="3"/>
         <v>3.831</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="4">
         <f t="shared" si="4"/>
         <v>5.9549999999999983</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="4">
         <f t="shared" si="5"/>
         <v>3.831</v>
       </c>
@@ -1333,33 +1354,33 @@
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>4.3</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>3.831</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <f t="shared" si="0"/>
         <v>4.82</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>3.831</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="4">
         <f t="shared" si="2"/>
         <v>5.34</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="4">
         <f t="shared" si="3"/>
         <v>3.831</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="4">
         <f t="shared" si="4"/>
         <v>5.8599999999999994</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="4">
         <f t="shared" si="5"/>
         <v>3.831</v>
       </c>
@@ -1368,33 +1389,33 @@
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>4.3470000000000004</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>3.6139999999999999</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <f t="shared" si="0"/>
         <v>4.8670000000000009</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <f t="shared" si="1"/>
         <v>3.6139999999999999</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="4">
         <f t="shared" si="2"/>
         <v>5.3870000000000005</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="4">
         <f t="shared" si="3"/>
         <v>3.6139999999999999</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="4">
         <f t="shared" si="4"/>
         <v>5.907</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="4">
         <f t="shared" si="5"/>
         <v>3.6139999999999999</v>
       </c>
@@ -1403,35 +1424,108 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>4.3470000000000004</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>3.5649999999999999</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <f t="shared" si="0"/>
         <v>4.8670000000000009</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <f t="shared" si="1"/>
         <v>3.5649999999999999</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="4">
         <f t="shared" si="2"/>
         <v>5.3870000000000005</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="4">
         <f t="shared" si="3"/>
         <v>3.5649999999999999</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="4">
         <f t="shared" si="4"/>
         <v>5.907</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="4">
         <f t="shared" si="5"/>
         <v>3.5649999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="B24">
+        <v>0.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="B25" s="4">
+        <f>B24/25.4</f>
+        <v>1.968503937007874E-2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="B28" s="4">
+        <f>B27/25.4</f>
+        <v>3.937007874015748E-2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="B31">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="B32" s="4">
+        <f>B31/25.4</f>
+        <v>3.5433070866141736</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="4">
+        <f>B34/25.4</f>
+        <v>1.5748031496062993</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>